<commit_message>
Added daily_usage_graph.py.  Modified DailyUsageDataFactory and DailyUsageData classes in usage_data.py
</commit_message>
<xml_diff>
--- a/data/temp-data.xlsx
+++ b/data/temp-data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -32,6 +32,81 @@
   </si>
   <si>
     <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-10-31</t>
   </si>
   <si>
     <t xml:space="preserve">2023-11-01</t>
@@ -164,6 +239,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,6 +260,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,7 +305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,6 +318,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,6 +335,15 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -258,13 +352,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -285,17 +379,17 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>33</v>
+      <c r="B2" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>52</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>63.5</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -303,17 +397,17 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>31</v>
+      <c r="B3" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>62</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -321,17 +415,17 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>40</v>
+      <c r="B4" s="4" t="n">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>63</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -339,17 +433,17 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>56</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>47.5</v>
+      <c r="B5" s="4" t="n">
+        <v>77</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>65</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -357,17 +451,17 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>56</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>46</v>
+      <c r="B6" s="4" t="n">
+        <v>71</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>59.5</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -375,17 +469,17 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>39</v>
+      <c r="B7" s="4" t="n">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>63.5</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -393,17 +487,17 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="4" t="n">
         <v>63</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>53.5</v>
+      <c r="C8" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>52.5</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -411,17 +505,17 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>37.5</v>
+      <c r="B9" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44.5</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -429,17 +523,17 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>59</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>46</v>
+      <c r="B10" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>43.5</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -447,17 +541,17 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="B11" s="4" t="n">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>40</v>
+      <c r="D11" s="4" t="n">
+        <v>45</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -465,17 +559,17 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>36</v>
+      <c r="B12" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>50</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -483,17 +577,17 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>27.5</v>
+      <c r="B13" s="4" t="n">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>45</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -501,17 +595,17 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>30.5</v>
+      <c r="B14" s="4" t="n">
+        <v>56</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>45</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -519,17 +613,17 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>35</v>
+      <c r="B15" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>55</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -537,17 +631,17 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="4" t="n">
+        <v>54</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="n">
         <v>50</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>35.5</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -555,17 +649,17 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>46</v>
+      <c r="B17" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>42</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -573,17 +667,17 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>49.5</v>
+      <c r="B18" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>41.5</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -591,17 +685,17 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="n">
-        <v>53</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>41.5</v>
+      <c r="B19" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>45.5</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -609,17 +703,17 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="C20" s="4" t="n">
         <v>46</v>
       </c>
-      <c r="C20" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>36.5</v>
+      <c r="D20" s="4" t="n">
+        <v>59.5</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -627,17 +721,17 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>32</v>
+      <c r="B21" s="4" t="n">
+        <v>74</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>61.5</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -645,17 +739,17 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>31</v>
+      <c r="B22" s="4" t="n">
+        <v>73</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>63</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -663,17 +757,17 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>42</v>
+      <c r="B23" s="4" t="n">
+        <v>72</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>60.5</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -681,17 +775,17 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="C24" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="C24" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>37.5</v>
+      <c r="D24" s="4" t="n">
+        <v>45.5</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -699,17 +793,17 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>30</v>
+      <c r="B25" s="4" t="n">
+        <v>53</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>46</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -717,17 +811,17 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="4" t="n">
+        <v>43</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="D26" s="4" t="n">
         <v>37</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>28.5</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -742,10 +836,10 @@
         <v>40</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -757,13 +851,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -775,13 +869,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>24.5</v>
+        <v>40</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -793,13 +887,13 @@
         <v>32</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>21</v>
+        <v>47.5</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -811,13 +905,13 @@
         <v>33</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -829,13 +923,13 @@
         <v>34</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -847,13 +941,13 @@
         <v>35</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45.5</v>
+        <v>53.5</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -865,13 +959,13 @@
         <v>36</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>43</v>
+        <v>37.5</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -883,108 +977,558 @@
         <v>37</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>36.5</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="C36" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="C36" s="2" t="n">
-        <v>29</v>
-      </c>
       <c r="D36" s="2" t="n">
-        <v>31.5</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>26.5</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+        <v>27.5</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+        <v>30.5</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="B46" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="C61" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="D65" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>